<commit_message>
FAB-305: Update Tobi's excel doc
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/DataCleaningDocumentation/FeatureUIRequirements.xlsx
+++ b/Project supporting Artifacts/DataCleaningDocumentation/FeatureUIRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobi/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/DataCleaningDocumentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanmccrossan/group_project/TUD-Group-Project/Project supporting Artifacts/DataCleaningDocumentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAC8527-8B93-BF4A-893C-D6D57DD3E5F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E25C60-B545-9547-A59B-98CA72B91BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{9AF54E71-4E9A-423E-8A07-24112C831AAE}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="33600" windowHeight="20200" xr2:uid="{9AF54E71-4E9A-423E-8A07-24112C831AAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -594,9 +594,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -622,12 +629,24 @@
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -642,23 +661,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -976,39 +1020,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B14EF5D-2ACB-42D9-9638-CB157AEBDFAB}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I10" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="55" style="1" customWidth="1"/>
-    <col min="2" max="2" width="149.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="140.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="187.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="36.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="24.5" style="12" customWidth="1"/>
     <col min="6" max="6" width="24.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="29.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="93.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="178.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="31.1640625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="31.6640625" style="8" customWidth="1"/>
     <col min="11" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="12" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1020,7 +1064,7 @@
       <c r="H1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="9" t="s">
         <v>38</v>
       </c>
       <c r="J1" s="6" t="s">
@@ -1028,22 +1072,22 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="153" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -1052,7 +1096,7 @@
       <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="9" t="s">
         <v>39</v>
       </c>
       <c r="J2" s="7" t="s">
@@ -1060,51 +1104,51 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="204" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>7</v>
+      <c r="G3" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="10" t="s">
         <v>40</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="12" t="s">
         <v>22</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -1113,30 +1157,30 @@
       <c r="H4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="8" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -1145,7 +1189,7 @@
       <c r="H5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="10" t="s">
         <v>42</v>
       </c>
       <c r="J5" s="6" t="s">
@@ -1153,22 +1197,22 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="153" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -1177,27 +1221,27 @@
       <c r="H6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="10" t="s">
         <v>43</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="12" t="s">
         <v>48</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -1206,24 +1250,24 @@
       <c r="H7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="12" t="s">
         <v>54</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -1232,7 +1276,7 @@
       <c r="H8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="10" t="s">
         <v>55</v>
       </c>
       <c r="J8" s="6" t="s">
@@ -1240,22 +1284,22 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="119" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>66</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -1264,7 +1308,7 @@
       <c r="H9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="10" t="s">
         <v>62</v>
       </c>
       <c r="J9" s="6" t="s">
@@ -1272,22 +1316,22 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="102" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>67</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -1296,7 +1340,7 @@
       <c r="H10" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="10" t="s">
         <v>68</v>
       </c>
       <c r="J10" s="6" t="s">
@@ -1304,22 +1348,22 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="153" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>74</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -1328,7 +1372,7 @@
       <c r="H11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="9" t="s">
         <v>75</v>
       </c>
       <c r="J11" s="6" t="s">
@@ -1336,22 +1380,22 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -1360,27 +1404,27 @@
       <c r="H12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="10" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>85</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -1389,7 +1433,7 @@
       <c r="H13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="10" t="s">
         <v>86</v>
       </c>
       <c r="J13" s="6" t="s">
@@ -1397,22 +1441,22 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="136" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>92</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -1421,30 +1465,30 @@
       <c r="H14" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="10" t="s">
         <v>95</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>99</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -1453,7 +1497,7 @@
       <c r="H15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I15" s="9" t="s">
         <v>100</v>
       </c>
       <c r="J15" s="6" t="s">
@@ -1461,22 +1505,22 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="204" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>106</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -1485,27 +1529,27 @@
       <c r="H16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="9" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="153" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>109</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -1514,7 +1558,7 @@
       <c r="H17" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="9" t="s">
         <v>112</v>
       </c>
       <c r="J17" s="6" t="s">
@@ -1522,22 +1566,22 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="238" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G18" s="1" t="s">
@@ -1546,27 +1590,27 @@
       <c r="H18" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="11" t="s">
         <v>144</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="12" t="s">
         <v>124</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -1575,7 +1619,7 @@
       <c r="H19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I19" s="9" t="s">
         <v>125</v>
       </c>
       <c r="J19" s="6" t="s">
@@ -1583,31 +1627,31 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="136" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="4" t="s">
         <v>140</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="11" t="s">
         <v>145</v>
       </c>
       <c r="J20" s="6" t="s">

</xml_diff>